<commit_message>
dict based financial ratios cal; new functions
</commit_message>
<xml_diff>
--- a/DATA/dict_import_csv_R.xlsx
+++ b/DATA/dict_import_csv_R.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="17535" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38320" windowHeight="23540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bal_sheet" sheetId="1" r:id="rId1"/>
     <sheet name="cash_flow" sheetId="3" r:id="rId2"/>
     <sheet name="income_stat" sheetId="4" r:id="rId3"/>
+    <sheet name="dict_new_var" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bal_sheet!$A$1:$F$112</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="939">
   <si>
     <t>机构ID</t>
   </si>
@@ -2573,17 +2574,305 @@
   </si>
   <si>
     <t>PNL_F050N</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>gross_margin</t>
+  </si>
+  <si>
+    <t>gross_profit</t>
+  </si>
+  <si>
+    <t>毛利率</t>
+  </si>
+  <si>
+    <t>毛利</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>毛利／营业收入</t>
+  </si>
+  <si>
+    <t>营业收入 - 营业成本</t>
+  </si>
+  <si>
+    <t>Gross profit</t>
+  </si>
+  <si>
+    <t>Gross margin</t>
+  </si>
+  <si>
+    <t>PNL_F006N - PNL_F007N</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">gross_profit / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>PNL_F006N</t>
+    </r>
+  </si>
+  <si>
+    <t>net_profit_recur</t>
+  </si>
+  <si>
+    <t>扣非净利润</t>
+  </si>
+  <si>
+    <t>Net profit without non-recurring PnL</t>
+  </si>
+  <si>
+    <t>gross_profit - PNL_F008N - PNL_F009N - PNL_F010N - PNL_F011N - PNL_F012N - PNL_F013N + PNL_F016N - PNL_F025N</t>
+  </si>
+  <si>
+    <t>毛利 - 营业税 - 期间费用 - 资产减值 + 联营合营投资收益 -所得税</t>
+  </si>
+  <si>
+    <t>net_profit_recur / PNL_F006N</t>
+  </si>
+  <si>
+    <t>扣非净利润 / 营业收入</t>
+  </si>
+  <si>
+    <t>销售净利润率（扣非）</t>
+  </si>
+  <si>
+    <t>net_recur_profit_margin</t>
+  </si>
+  <si>
+    <t>Net margin (without non-recurring PnL)</t>
+  </si>
+  <si>
+    <t>总资产净利润率（扣非）</t>
+  </si>
+  <si>
+    <t>net_profit_recur / BAL_F038N</t>
+  </si>
+  <si>
+    <t>扣非净利润 / 总资产</t>
+  </si>
+  <si>
+    <t>roa_recur</t>
+  </si>
+  <si>
+    <t>ROA (without non-recurring PnL)</t>
+  </si>
+  <si>
+    <t>roe_recur</t>
+  </si>
+  <si>
+    <t>净资产收益率（扣非）</t>
+  </si>
+  <si>
+    <t>ROE (without non-recurring PnL)</t>
+  </si>
+  <si>
+    <t>扣非净利润(归属于母公司) / 净资产</t>
+  </si>
+  <si>
+    <t>盈利现金比率</t>
+  </si>
+  <si>
+    <t>销售现金比率</t>
+  </si>
+  <si>
+    <t>扣非净利润／净利润</t>
+  </si>
+  <si>
+    <t>net_op_cash_2_net_profit</t>
+  </si>
+  <si>
+    <t>cash_sales_2_op_income</t>
+  </si>
+  <si>
+    <t>net_profit_recur_2_net_profit</t>
+  </si>
+  <si>
+    <t>Earning cash ratio</t>
+  </si>
+  <si>
+    <t>Cash slaes ratio</t>
+  </si>
+  <si>
+    <t>经营性现金净流量 ／ 净利润</t>
+  </si>
+  <si>
+    <t>销售商品或提供劳务收到的现金 ／ 销售收入</t>
+  </si>
+  <si>
+    <t>CF_F015N / PNL_F027N</t>
+  </si>
+  <si>
+    <t>CF_F006N / PNL_F006N</t>
+  </si>
+  <si>
+    <t>net_profit_recur / PNL_F027N</t>
+  </si>
+  <si>
+    <t>sales_expense_2_op_income</t>
+  </si>
+  <si>
+    <t>admin_expense_2_op_income</t>
+  </si>
+  <si>
+    <t>finance_expense_2_op_income</t>
+  </si>
+  <si>
+    <t>销售费用率</t>
+  </si>
+  <si>
+    <t>管理费用率</t>
+  </si>
+  <si>
+    <t>财务费用率</t>
+  </si>
+  <si>
+    <t>Sales expense margin</t>
+  </si>
+  <si>
+    <t>Admin expense margin</t>
+  </si>
+  <si>
+    <t>Finan expense margin</t>
+  </si>
+  <si>
+    <t>PNL_F009N / PNL_F006N</t>
+  </si>
+  <si>
+    <t>PNL_F010N / PNL_F006N</t>
+  </si>
+  <si>
+    <t>PNL_F012N / PNL_F006N</t>
+  </si>
+  <si>
+    <t>销售费用 ／ 销售收入</t>
+  </si>
+  <si>
+    <t>管理费用 ／ 销售收入</t>
+  </si>
+  <si>
+    <t>财务费用 ／ 销售收入</t>
+  </si>
+  <si>
+    <t>经营活动产生的现金流净额 — 投资活动产生的现金流净额</t>
+  </si>
+  <si>
+    <t>Net recurring profit / net profit</t>
+  </si>
+  <si>
+    <t>Free cash flow</t>
+  </si>
+  <si>
+    <t>CF_F015N - CF_F027N</t>
+  </si>
+  <si>
+    <t>自由现金流</t>
+  </si>
+  <si>
+    <t>free_cash_flow</t>
+  </si>
+  <si>
+    <t>quick_ratio</t>
+  </si>
+  <si>
+    <t>速度比率</t>
+  </si>
+  <si>
+    <t>(流动资产 — 存货 — 预付账款)/流动负债</t>
+  </si>
+  <si>
+    <t>Quick ratio</t>
+  </si>
+  <si>
+    <t>current_ratio</t>
+  </si>
+  <si>
+    <t>流动比率</t>
+  </si>
+  <si>
+    <t>流动资产 ／ 流动负债</t>
+  </si>
+  <si>
+    <t>Current ratio</t>
+  </si>
+  <si>
+    <t>BAL_F019N / BAL_F052N</t>
+  </si>
+  <si>
+    <t>现金流量比率</t>
+  </si>
+  <si>
+    <t>net_op_cash_2_current_liab</t>
+  </si>
+  <si>
+    <t>Net op cash to current liab</t>
+  </si>
+  <si>
+    <t>经营活动现金净流量 ／ 流动负债</t>
+  </si>
+  <si>
+    <t>CF_F015N / BAL_F052N</t>
+  </si>
+  <si>
+    <t>asset_2_liab</t>
+  </si>
+  <si>
+    <t>资产负债率</t>
+  </si>
+  <si>
+    <t>负债总额 ／ 资产总额</t>
+  </si>
+  <si>
+    <t>BAL_F038N / BAL_F070N</t>
+  </si>
+  <si>
+    <t>Asset-to-equity ratio</t>
+  </si>
+  <si>
+    <t>Liability to Asset ratio</t>
+  </si>
+  <si>
+    <t>BAL_F061N / BAL_F038N</t>
+  </si>
+  <si>
+    <t>权益乘数</t>
+  </si>
+  <si>
+    <t>asset_2_equity</t>
+  </si>
+  <si>
+    <t>总资产 ／ 股东权益</t>
+  </si>
+  <si>
+    <t>PNL_F028N / PNL_F027N * net_profit_recur / BAL_F070N</t>
+  </si>
+  <si>
+    <t>(BAL_F019N - BAL_F015N - BAL_F010N)/BAL_F052N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2591,7 +2880,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2599,7 +2888,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2607,15 +2896,30 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2636,7 +2940,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2678,53 +2982,224 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="41">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+  <cellStyles count="123">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -3052,19 +3527,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="45.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="50.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5614,7 +6089,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5624,14 +6099,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
@@ -7817,19 +8292,24 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
@@ -9153,5 +9633,420 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" customWidth="1"/>
+    <col min="6" max="6" width="63.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>849</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="C2" t="s">
+        <v>856</v>
+      </c>
+      <c r="D2" t="s">
+        <v>858</v>
+      </c>
+      <c r="E2" t="s">
+        <v>430</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>848</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="C3" t="s">
+        <v>857</v>
+      </c>
+      <c r="D3" t="s">
+        <v>859</v>
+      </c>
+      <c r="E3" t="s">
+        <v>853</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>860</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="C4" t="s">
+        <v>862</v>
+      </c>
+      <c r="D4" t="s">
+        <v>863</v>
+      </c>
+      <c r="E4" t="s">
+        <v>430</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>868</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="C5" t="s">
+        <v>869</v>
+      </c>
+      <c r="D5" t="s">
+        <v>865</v>
+      </c>
+      <c r="E5" t="s">
+        <v>853</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>873</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="C6" t="s">
+        <v>874</v>
+      </c>
+      <c r="D6" t="s">
+        <v>871</v>
+      </c>
+      <c r="E6" t="s">
+        <v>853</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>875</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="C7" t="s">
+        <v>877</v>
+      </c>
+      <c r="D7" t="s">
+        <v>937</v>
+      </c>
+      <c r="E7" t="s">
+        <v>853</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>892</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="C8" t="s">
+        <v>898</v>
+      </c>
+      <c r="D8" t="s">
+        <v>901</v>
+      </c>
+      <c r="E8" t="s">
+        <v>853</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>893</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="C9" t="s">
+        <v>899</v>
+      </c>
+      <c r="D9" t="s">
+        <v>902</v>
+      </c>
+      <c r="E9" t="s">
+        <v>853</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>894</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="C10" t="s">
+        <v>900</v>
+      </c>
+      <c r="D10" t="s">
+        <v>903</v>
+      </c>
+      <c r="E10" t="s">
+        <v>853</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>882</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="C11" t="s">
+        <v>885</v>
+      </c>
+      <c r="D11" t="s">
+        <v>889</v>
+      </c>
+      <c r="E11" t="s">
+        <v>853</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>883</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="C12" t="s">
+        <v>886</v>
+      </c>
+      <c r="D12" t="s">
+        <v>890</v>
+      </c>
+      <c r="E12" t="s">
+        <v>853</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>884</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="C13" t="s">
+        <v>908</v>
+      </c>
+      <c r="D13" t="s">
+        <v>891</v>
+      </c>
+      <c r="E13" t="s">
+        <v>853</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>912</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="C14" t="s">
+        <v>909</v>
+      </c>
+      <c r="D14" t="s">
+        <v>910</v>
+      </c>
+      <c r="E14" t="s">
+        <v>430</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>913</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="C15" t="s">
+        <v>916</v>
+      </c>
+      <c r="D15" t="s">
+        <v>938</v>
+      </c>
+      <c r="E15" t="s">
+        <v>853</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>917</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="C16" t="s">
+        <v>920</v>
+      </c>
+      <c r="D16" t="s">
+        <v>921</v>
+      </c>
+      <c r="E16" t="s">
+        <v>853</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>923</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="C17" t="s">
+        <v>924</v>
+      </c>
+      <c r="D17" t="s">
+        <v>926</v>
+      </c>
+      <c r="E17" t="s">
+        <v>853</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>927</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="C18" t="s">
+        <v>932</v>
+      </c>
+      <c r="D18" t="s">
+        <v>933</v>
+      </c>
+      <c r="E18" t="s">
+        <v>853</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>935</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="C19" t="s">
+        <v>931</v>
+      </c>
+      <c r="D19" t="s">
+        <v>930</v>
+      </c>
+      <c r="E19" t="s">
+        <v>853</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
py code for collecting data from API; update template
</commit_message>
<xml_diff>
--- a/DATA/dict_import_csv_R.xlsx
+++ b/DATA/dict_import_csv_R.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38320" windowHeight="23540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="35000" yWindow="-660" windowWidth="38320" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="bal_sheet" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="943">
   <si>
     <t>机构ID</t>
   </si>
@@ -2862,6 +2862,18 @@
   </si>
   <si>
     <t>(BAL_F019N - BAL_F015N - BAL_F010N)/BAL_F052N</t>
+  </si>
+  <si>
+    <t>BAL_MEMO</t>
+  </si>
+  <si>
+    <t>CF_MEMO</t>
+  </si>
+  <si>
+    <t>PNL_MEMO</t>
+  </si>
+  <si>
+    <t>PNL_F051N</t>
   </si>
 </sst>
 </file>
@@ -2940,8 +2952,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="123">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3076,7 +3090,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="123">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3138,6 +3152,7 @@
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3199,6 +3214,7 @@
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3530,8 +3546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6071,7 +6087,7 @@
         <v>249</v>
       </c>
       <c r="B112" t="s">
-        <v>248</v>
+        <v>939</v>
       </c>
       <c r="C112" t="s">
         <v>248</v>
@@ -6100,10 +6116,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8287,6 +8303,26 @@
       </c>
       <c r="G96" t="s">
         <v>561</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>249</v>
+      </c>
+      <c r="B97" t="s">
+        <v>940</v>
+      </c>
+      <c r="C97" t="s">
+        <v>248</v>
+      </c>
+      <c r="D97" t="s">
+        <v>249</v>
+      </c>
+      <c r="E97" t="s">
+        <v>431</v>
+      </c>
+      <c r="G97" t="s">
+        <v>609</v>
       </c>
     </row>
   </sheetData>
@@ -8305,8 +8341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9592,7 +9628,7 @@
         <v>249</v>
       </c>
       <c r="B57" t="s">
-        <v>248</v>
+        <v>941</v>
       </c>
       <c r="C57" t="s">
         <v>248</v>
@@ -9612,7 +9648,7 @@
         <v>606</v>
       </c>
       <c r="B58" t="s">
-        <v>200</v>
+        <v>942</v>
       </c>
       <c r="C58" t="s">
         <v>200</v>
@@ -9646,7 +9682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update sqlite with API feeded data
</commit_message>
<xml_diff>
--- a/DATA/dict_import_csv_R.xlsx
+++ b/DATA/dict_import_csv_R.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="35000" yWindow="-660" windowWidth="38320" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="38320" yWindow="-1540" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bal_sheet" sheetId="1" r:id="rId1"/>
     <sheet name="cash_flow" sheetId="3" r:id="rId2"/>
     <sheet name="income_stat" sheetId="4" r:id="rId3"/>
-    <sheet name="dict_new_var" sheetId="5" r:id="rId4"/>
+    <sheet name="key_indi" sheetId="6" r:id="rId4"/>
+    <sheet name="dict_new_var" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bal_sheet!$A$1:$F$112</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2750" uniqueCount="1240">
   <si>
     <t>机构ID</t>
   </si>
@@ -2874,6 +2875,897 @@
   </si>
   <si>
     <t>PNL_F051N</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>F069D</t>
+  </si>
+  <si>
+    <t>YYYY-03-31: Q1 Report; YYYY-06-30: Interim Report; YYYY-09-30: Q3 Report; YYYY-12-31: Annual Report</t>
+  </si>
+  <si>
+    <t>F070V</t>
+  </si>
+  <si>
+    <t>F071V</t>
+  </si>
+  <si>
+    <t>F001V</t>
+  </si>
+  <si>
+    <t>Data Source Code</t>
+  </si>
+  <si>
+    <t>Data Source</t>
+  </si>
+  <si>
+    <t>F003N</t>
+  </si>
+  <si>
+    <t>EPS</t>
+  </si>
+  <si>
+    <t>DECIMAL</t>
+  </si>
+  <si>
+    <t>EPS: Earnings per Share</t>
+  </si>
+  <si>
+    <t>F004N</t>
+  </si>
+  <si>
+    <t>Basic EPS</t>
+  </si>
+  <si>
+    <t>F005N</t>
+  </si>
+  <si>
+    <t>Diluted EPS</t>
+  </si>
+  <si>
+    <t>EPS after Deducting Non-recurring Gains and Losses</t>
+  </si>
+  <si>
+    <t>Retained Profit Per Share</t>
+  </si>
+  <si>
+    <t>Net Asset Per Share</t>
+  </si>
+  <si>
+    <t>Adjusted Net Asset Per Share</t>
+  </si>
+  <si>
+    <t>Capital Reserve Per Share</t>
+  </si>
+  <si>
+    <t>Operating Profit Ratio</t>
+  </si>
+  <si>
+    <t>Operating Profit/ Operating Income*100</t>
+  </si>
+  <si>
+    <t>Operating Tax Ratio</t>
+  </si>
+  <si>
+    <t>Operating Taxes/ Operating Income*100</t>
+  </si>
+  <si>
+    <t>Operating Cost Ratio</t>
+  </si>
+  <si>
+    <t>Operating Cost/ Operating Income*100</t>
+  </si>
+  <si>
+    <t>ROE</t>
+  </si>
+  <si>
+    <t>ROE: Return on Equity, Net Income/Total Equity*100</t>
+  </si>
+  <si>
+    <t>ROI</t>
+  </si>
+  <si>
+    <t>ROI: Return on Investment, Investment Income / ( Held for Trading Financial Assets + Financial Assets Available for Sales+ Held-to-Maturity Investment)+ Long-term Equity Investment)* 100</t>
+  </si>
+  <si>
+    <t>ROA</t>
+  </si>
+  <si>
+    <t>ROA: Return on Assets, Net Profit/(Ending Total Assets+Beginning Total Assets)/2*100</t>
+  </si>
+  <si>
+    <t>Net Profit Ratio</t>
+  </si>
+  <si>
+    <t>Net Profit/ Operating Income * 100</t>
+  </si>
+  <si>
+    <t>Operating Expenses Ratio</t>
+  </si>
+  <si>
+    <t>Administrative Expense/ Operating Income * 100</t>
+  </si>
+  <si>
+    <t>Financial Expenses Ratio</t>
+  </si>
+  <si>
+    <t>Financial Expenses/ Operating Income* 100</t>
+  </si>
+  <si>
+    <t>Ratio of Profits to Cost</t>
+  </si>
+  <si>
+    <t>Total Profit/Total Cost×100</t>
+  </si>
+  <si>
+    <t>Proportion of Financial, Administrative and Operating Expenses</t>
+  </si>
+  <si>
+    <t>(Financial Expense+Administrative Expense+Operating Expense)/Operating Income*100</t>
+  </si>
+  <si>
+    <t>Receivables Turnover Ratio</t>
+  </si>
+  <si>
+    <t>Operating Income/ (Beginning Receivables + Ending Receivables)/ 2</t>
+  </si>
+  <si>
+    <t>Inventory Turnover Ratio</t>
+  </si>
+  <si>
+    <t>Operating Cost/ (Beginning Inventory+ Ending Inventory)/ 2</t>
+  </si>
+  <si>
+    <t>Turnover Ratio of Operating Funds</t>
+  </si>
+  <si>
+    <t>Operating Income/ (Beginning Current Assets - Beginning Current Liabilities) + (Ending Current Assets + Ending Current Liabilities) / 2</t>
+  </si>
+  <si>
+    <t>Total Assets Turnover Ratio</t>
+  </si>
+  <si>
+    <t>Operating Income / ((Beginning Total Assets + Ending Total Assets) / 2)</t>
+  </si>
+  <si>
+    <t>Fixed Assets Turnover Ratio</t>
+  </si>
+  <si>
+    <t>Operating Income/ ((Beginning Fixed Assets + Ending Fixed Assets) / 2)</t>
+  </si>
+  <si>
+    <t>Receivables Turnover Days</t>
+  </si>
+  <si>
+    <t>360/Receivables Turnover Ratio or (Beginning Receivables+Ending Receivables)/2] / Operating Income</t>
+  </si>
+  <si>
+    <t>Inventory Turnover Days</t>
+  </si>
+  <si>
+    <t>360/InventoryTurnover; InventoryTurnover=[360*(Beginning Inventory + Ending Inventory)/2]/ Operating Cost</t>
+  </si>
+  <si>
+    <t>Current Assets Turnover</t>
+  </si>
+  <si>
+    <t>Operating Income/[(Beginning Current Assets+Ending Current Assets)/2]</t>
+  </si>
+  <si>
+    <t>Current Assets Turnover Days</t>
+  </si>
+  <si>
+    <t>360/Current Assets Turnover</t>
+  </si>
+  <si>
+    <t>Total Assets Turnover Days</t>
+  </si>
+  <si>
+    <t>360/ Total Assets Turnover</t>
+  </si>
+  <si>
+    <t>Equity Turnover</t>
+  </si>
+  <si>
+    <t>Operating Income*2/(Beginning Shareholders’ Equity+ Ending Shareholders’ Equity)</t>
+  </si>
+  <si>
+    <t>Current Assets Ratio</t>
+  </si>
+  <si>
+    <t>Current Assets/Total Assets*100</t>
+  </si>
+  <si>
+    <t>Monetary Fund Ratio</t>
+  </si>
+  <si>
+    <t>Monetary Fund /Current Assets*100</t>
+  </si>
+  <si>
+    <t>Trading Financial Assets Ratio</t>
+  </si>
+  <si>
+    <t>Short-term Investment/Current Assets*100</t>
+  </si>
+  <si>
+    <t>Inventory Ratio</t>
+  </si>
+  <si>
+    <t>Inventory/Current Assets*100</t>
+  </si>
+  <si>
+    <t>Fixed Assets Ratio</t>
+  </si>
+  <si>
+    <t>Fixed Assets/Total Assets*100</t>
+  </si>
+  <si>
+    <t>Liability Structure Ratio</t>
+  </si>
+  <si>
+    <t>Current Liabilities/Non-current Liabilities*100</t>
+  </si>
+  <si>
+    <t>Equity Ratio</t>
+  </si>
+  <si>
+    <t>Total Liabilities/Shareholders’ Equity*100</t>
+  </si>
+  <si>
+    <t>Net Assets Ratio</t>
+  </si>
+  <si>
+    <t>100- Ratio of Debts to Assets; Net Asset/Total Assets*100</t>
+  </si>
+  <si>
+    <t>Asset Liability Ratio</t>
+  </si>
+  <si>
+    <t>Total Liabilities / Total Assets * 100</t>
+  </si>
+  <si>
+    <t>Current Ratio</t>
+  </si>
+  <si>
+    <t>Current Assets/ Current Liabilities</t>
+  </si>
+  <si>
+    <t>Quick Ratio</t>
+  </si>
+  <si>
+    <t>(Current Assets- Inventory)/ Current Liabilities</t>
+  </si>
+  <si>
+    <t>Cash Asset Ratio</t>
+  </si>
+  <si>
+    <t>Monetary Fund /Current Liabilities*100</t>
+  </si>
+  <si>
+    <t>Working Capital</t>
+  </si>
+  <si>
+    <t>Current Assets-Current Liabilities</t>
+  </si>
+  <si>
+    <t>Non-current Debt Ratio</t>
+  </si>
+  <si>
+    <t>(Non-current Liabilities / Total Liabilities) * 100</t>
+  </si>
+  <si>
+    <t>Current Debt Ratio</t>
+  </si>
+  <si>
+    <t>Current Liabilities / Total Liabilities * 100</t>
+  </si>
+  <si>
+    <t>Conservative Quick Ratio</t>
+  </si>
+  <si>
+    <t>Monetary Fund + Held for Trading Financial Assets + Notes Receivables + Receivables + Other Receivable ) / Current Liabilities, Acid Ratio</t>
+  </si>
+  <si>
+    <t>Cash-due Debt Ratio</t>
+  </si>
+  <si>
+    <t>Net Cash Provided by Operating Activities * 100 / Current Due Debts = Net Cash Provided by Operating Activities * 100/(Current Maturities of Non-current Liabilities＋Notes Payable)</t>
+  </si>
+  <si>
+    <t>Debt to Tangible Assets Ratio</t>
+  </si>
+  <si>
+    <t>Current Liabilities/(Shareholders’ Equity-Intangible Asset)</t>
+  </si>
+  <si>
+    <t>Operating Income Growth Rate</t>
+  </si>
+  <si>
+    <t>(Current Operating Income /Previous Operating Income -1)*100</t>
+  </si>
+  <si>
+    <t>Net Profit Growth Rate</t>
+  </si>
+  <si>
+    <t>(Current Net Profit /Previous Net Profit -1)*100 (Ending Shareholders' Equity/Beginning Shareholders' Equity-1)*100</t>
+  </si>
+  <si>
+    <t>Net Assets Growth Rate</t>
+  </si>
+  <si>
+    <t>(Ending Shareholders’ Equity/Beginning Shareholders’ Equity-1)*100</t>
+  </si>
+  <si>
+    <t>Fixed Assets Growth Rate</t>
+  </si>
+  <si>
+    <t>(Ending Fixed Assets/Beginning Fixed Assets-1)*100</t>
+  </si>
+  <si>
+    <t>Total Assets Growth Rate</t>
+  </si>
+  <si>
+    <t>(Ending Total Assets/Beginning Total Assets-1)*100</t>
+  </si>
+  <si>
+    <t>Investment Income Growth Rate</t>
+  </si>
+  <si>
+    <t>(Current Investment Income /Previous Investment Income -1)*100</t>
+  </si>
+  <si>
+    <t>Operating Profit Growth Rate</t>
+  </si>
+  <si>
+    <t>(Current Operating Profit /Previous Operating Profit -1)*100</t>
+  </si>
+  <si>
+    <t>Cash Flow Per Share</t>
+  </si>
+  <si>
+    <t>Net Cash Flow/Share Capital</t>
+  </si>
+  <si>
+    <t>Operating Cash Flow Per Share</t>
+  </si>
+  <si>
+    <t>Net Cash Provided by Operating Activities/Share Capital</t>
+  </si>
+  <si>
+    <t>Operating Net Cash Ratio(Short-term Debts)</t>
+  </si>
+  <si>
+    <t>Net Cash Provided by Operating Activities *100/Current Liabilities</t>
+  </si>
+  <si>
+    <t>Operating Net Cash Ratio(Total Debts)</t>
+  </si>
+  <si>
+    <t>Net Cash Provided by Operating Activities *100/Total Liabilities</t>
+  </si>
+  <si>
+    <t>Net Cash Provided by Operating Activities to Net Profit</t>
+  </si>
+  <si>
+    <t>Net Cash Provided by Operating Activities*100/Net Profit</t>
+  </si>
+  <si>
+    <t>Operating Income Cash Coverage</t>
+  </si>
+  <si>
+    <t>Cash Inflow from Operating Activities*100/Operating Income</t>
+  </si>
+  <si>
+    <t>Cash Recovery for All Assets</t>
+  </si>
+  <si>
+    <t>Net Cash Provided by Operating Activities *100 /Total Assets</t>
+  </si>
+  <si>
+    <t>ROE after Deducting Non-recurring Gains and Losses</t>
+  </si>
+  <si>
+    <t>ROE: Return on Equity</t>
+  </si>
+  <si>
+    <t>Weighted ROE</t>
+  </si>
+  <si>
+    <t>Weighted ROE after Deducting Non-recurring Gains and Losses</t>
+  </si>
+  <si>
+    <t>Net profit after Deducting Non Recurring Gains and Losses</t>
+  </si>
+  <si>
+    <t>Total Non Recurring Gains and Losses</t>
+  </si>
+  <si>
+    <t>INDI_F001V</t>
+  </si>
+  <si>
+    <t>INDI_F002V</t>
+  </si>
+  <si>
+    <t>INDI_F003N</t>
+  </si>
+  <si>
+    <t>INDI_F004N</t>
+  </si>
+  <si>
+    <t>INDI_F005N</t>
+  </si>
+  <si>
+    <t>INDI_F006N</t>
+  </si>
+  <si>
+    <t>INDI_F007N</t>
+  </si>
+  <si>
+    <t>INDI_F008N</t>
+  </si>
+  <si>
+    <t>INDI_F009N</t>
+  </si>
+  <si>
+    <t>INDI_F010N</t>
+  </si>
+  <si>
+    <t>INDI_F011N</t>
+  </si>
+  <si>
+    <t>INDI_F012N</t>
+  </si>
+  <si>
+    <t>INDI_F013N</t>
+  </si>
+  <si>
+    <t>INDI_F014N</t>
+  </si>
+  <si>
+    <t>INDI_F015N</t>
+  </si>
+  <si>
+    <t>INDI_F016N</t>
+  </si>
+  <si>
+    <t>INDI_F017N</t>
+  </si>
+  <si>
+    <t>INDI_F018N</t>
+  </si>
+  <si>
+    <t>INDI_F019N</t>
+  </si>
+  <si>
+    <t>INDI_F020N</t>
+  </si>
+  <si>
+    <t>INDI_F021N</t>
+  </si>
+  <si>
+    <t>INDI_F022N</t>
+  </si>
+  <si>
+    <t>INDI_F023N</t>
+  </si>
+  <si>
+    <t>INDI_F024N</t>
+  </si>
+  <si>
+    <t>INDI_F025N</t>
+  </si>
+  <si>
+    <t>INDI_F026N</t>
+  </si>
+  <si>
+    <t>INDI_F027N</t>
+  </si>
+  <si>
+    <t>INDI_F028N</t>
+  </si>
+  <si>
+    <t>INDI_F029N</t>
+  </si>
+  <si>
+    <t>INDI_F030N</t>
+  </si>
+  <si>
+    <t>INDI_F031N</t>
+  </si>
+  <si>
+    <t>INDI_F032N</t>
+  </si>
+  <si>
+    <t>INDI_F033N</t>
+  </si>
+  <si>
+    <t>INDI_F034N</t>
+  </si>
+  <si>
+    <t>INDI_F035N</t>
+  </si>
+  <si>
+    <t>INDI_F036N</t>
+  </si>
+  <si>
+    <t>INDI_F037N</t>
+  </si>
+  <si>
+    <t>INDI_F038N</t>
+  </si>
+  <si>
+    <t>INDI_F039N</t>
+  </si>
+  <si>
+    <t>INDI_F040N</t>
+  </si>
+  <si>
+    <t>INDI_F041N</t>
+  </si>
+  <si>
+    <t>INDI_F042N</t>
+  </si>
+  <si>
+    <t>INDI_F043N</t>
+  </si>
+  <si>
+    <t>INDI_F044N</t>
+  </si>
+  <si>
+    <t>INDI_F046N</t>
+  </si>
+  <si>
+    <t>INDI_F047N</t>
+  </si>
+  <si>
+    <t>INDI_F048N</t>
+  </si>
+  <si>
+    <t>INDI_F049N</t>
+  </si>
+  <si>
+    <t>INDI_F050N</t>
+  </si>
+  <si>
+    <t>INDI_F051N</t>
+  </si>
+  <si>
+    <t>INDI_F052N</t>
+  </si>
+  <si>
+    <t>INDI_F053N</t>
+  </si>
+  <si>
+    <t>INDI_F054N</t>
+  </si>
+  <si>
+    <t>INDI_F055N</t>
+  </si>
+  <si>
+    <t>INDI_F056N</t>
+  </si>
+  <si>
+    <t>INDI_F057N</t>
+  </si>
+  <si>
+    <t>INDI_F058N</t>
+  </si>
+  <si>
+    <t>INDI_F059N</t>
+  </si>
+  <si>
+    <t>INDI_F060N</t>
+  </si>
+  <si>
+    <t>INDI_F061N</t>
+  </si>
+  <si>
+    <t>INDI_F062N</t>
+  </si>
+  <si>
+    <t>INDI_F063N</t>
+  </si>
+  <si>
+    <t>INDI_F064N</t>
+  </si>
+  <si>
+    <t>INDI_F065N</t>
+  </si>
+  <si>
+    <t>INDI_F066N</t>
+  </si>
+  <si>
+    <t>INDI_F067N</t>
+  </si>
+  <si>
+    <t>INDI_F068N</t>
+  </si>
+  <si>
+    <t>INDI_F076N</t>
+  </si>
+  <si>
+    <t>INDI_F077N</t>
+  </si>
+  <si>
+    <t>数据来源编码</t>
+  </si>
+  <si>
+    <t>数据来源</t>
+  </si>
+  <si>
+    <t>每股收益</t>
+  </si>
+  <si>
+    <t>基本每股收益</t>
+  </si>
+  <si>
+    <t>稀释每股收益</t>
+  </si>
+  <si>
+    <t>扣除非经常性损益每股收益</t>
+  </si>
+  <si>
+    <t>每股未分配利润</t>
+  </si>
+  <si>
+    <t>每股净资产</t>
+  </si>
+  <si>
+    <t>调整后每股净资产</t>
+  </si>
+  <si>
+    <t>每股资本公积金</t>
+  </si>
+  <si>
+    <t>营业利润率</t>
+  </si>
+  <si>
+    <t>营业税金率</t>
+  </si>
+  <si>
+    <t>营业成本率</t>
+  </si>
+  <si>
+    <t>净资产收益率</t>
+  </si>
+  <si>
+    <t>投资收益率</t>
+  </si>
+  <si>
+    <t>总资产报酬率</t>
+  </si>
+  <si>
+    <t>净利润率</t>
+  </si>
+  <si>
+    <t>成本费用利润率</t>
+  </si>
+  <si>
+    <t>三费比重</t>
+  </si>
+  <si>
+    <t>应收账款周转率</t>
+  </si>
+  <si>
+    <t>存货周转率</t>
+  </si>
+  <si>
+    <t>运营资金周转率</t>
+  </si>
+  <si>
+    <t>总资产周转率</t>
+  </si>
+  <si>
+    <t>固定资产周转率</t>
+  </si>
+  <si>
+    <t>应收账款周转天数</t>
+  </si>
+  <si>
+    <t>存货周转天数</t>
+  </si>
+  <si>
+    <t>流动资产周转率</t>
+  </si>
+  <si>
+    <t>流动资产周转天数</t>
+  </si>
+  <si>
+    <t>总资产周转天数</t>
+  </si>
+  <si>
+    <t>股东权益周转率</t>
+  </si>
+  <si>
+    <t>流动资产比率</t>
+  </si>
+  <si>
+    <t>货币资金比率</t>
+  </si>
+  <si>
+    <t>交易性金融资产比率</t>
+  </si>
+  <si>
+    <t>存货比率</t>
+  </si>
+  <si>
+    <t>固定资产比率</t>
+  </si>
+  <si>
+    <t>负债结构比</t>
+  </si>
+  <si>
+    <t>产权比率</t>
+  </si>
+  <si>
+    <t>净资产比率</t>
+  </si>
+  <si>
+    <t>资产负债比率</t>
+  </si>
+  <si>
+    <t>速动比率</t>
+  </si>
+  <si>
+    <t>现金比率</t>
+  </si>
+  <si>
+    <t>利息保障倍数</t>
+  </si>
+  <si>
+    <t>息税前利润/利息费用=(利润总额+财务费用)/财务费用</t>
+  </si>
+  <si>
+    <t>营运资金</t>
+  </si>
+  <si>
+    <t>非流动负债比率</t>
+  </si>
+  <si>
+    <t>流动负债比率</t>
+  </si>
+  <si>
+    <t>保守速动比率</t>
+  </si>
+  <si>
+    <t>现金到期债务比率</t>
+  </si>
+  <si>
+    <t>有形资产净值债务率</t>
+  </si>
+  <si>
+    <t>营业收入增长率</t>
+  </si>
+  <si>
+    <t>净利润增长率</t>
+  </si>
+  <si>
+    <t>净资产增长率</t>
+  </si>
+  <si>
+    <t>固定资产增长率</t>
+  </si>
+  <si>
+    <t>总资产增长率</t>
+  </si>
+  <si>
+    <t>投资收益增长率</t>
+  </si>
+  <si>
+    <t>营业利润增长率</t>
+  </si>
+  <si>
+    <t>每股现金流量</t>
+  </si>
+  <si>
+    <t>每股经营现金流量</t>
+  </si>
+  <si>
+    <t>经营净现金比率（短期债务）</t>
+  </si>
+  <si>
+    <t>经营净现金比率（全部债务）</t>
+  </si>
+  <si>
+    <t>经营活动现金净流量与净利润比率</t>
+  </si>
+  <si>
+    <t>营业收入现金含量</t>
+  </si>
+  <si>
+    <t>全部资产现金回收率</t>
+  </si>
+  <si>
+    <t>净资产收益率(扣除非经常性损益)</t>
+  </si>
+  <si>
+    <t>净资产收益率-加权</t>
+  </si>
+  <si>
+    <t>净资产收益率-加权(扣除非经常性损益)</t>
+  </si>
+  <si>
+    <t>扣除非经常性损益后的净利润</t>
+  </si>
+  <si>
+    <t>非经常性损益合计</t>
+  </si>
+  <si>
+    <t>期间费用率</t>
+  </si>
+  <si>
+    <t>现金转换周期</t>
+  </si>
+  <si>
+    <t>净利含金量</t>
+  </si>
+  <si>
+    <t>非经常性损益占比</t>
+  </si>
+  <si>
+    <t>期间费用增长率</t>
+  </si>
+  <si>
+    <t>基本获利能力</t>
+  </si>
+  <si>
+    <t>应收账款占比</t>
+  </si>
+  <si>
+    <t>存货占比</t>
+  </si>
+  <si>
+    <t>年化期间费用毛利比</t>
+  </si>
+  <si>
+    <t>desc_en</t>
+  </si>
+  <si>
+    <t>desc_cn</t>
+  </si>
+  <si>
+    <t>INDI_F078N</t>
+  </si>
+  <si>
+    <t>INDI_F079N</t>
+  </si>
+  <si>
+    <t>INDI_F080N</t>
+  </si>
+  <si>
+    <t>INDI_F081N</t>
+  </si>
+  <si>
+    <t>INDI_F082N</t>
+  </si>
+  <si>
+    <t>INDI_F083N</t>
+  </si>
+  <si>
+    <t>INDI_F084N</t>
+  </si>
+  <si>
+    <t>INDI_F085N</t>
+  </si>
+  <si>
+    <t>INDI_F086N</t>
+  </si>
+  <si>
+    <t>INDI_F087N</t>
+  </si>
+  <si>
+    <t>INDI_F088N</t>
+  </si>
+  <si>
+    <t>INDI_F045N</t>
+  </si>
+  <si>
+    <t>Gross Margin</t>
   </si>
 </sst>
 </file>
@@ -2952,8 +3844,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="125">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3090,7 +4030,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="125">
+  <cellStyles count="173">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3153,6 +4093,30 @@
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3215,6 +4179,30 @@
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3546,8 +4534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110:G111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6116,10 +7104,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8323,6 +9311,46 @@
       </c>
       <c r="G97" t="s">
         <v>609</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" t="s">
+        <v>95</v>
+      </c>
+      <c r="B98" t="s">
+        <v>94</v>
+      </c>
+      <c r="C98" t="s">
+        <v>94</v>
+      </c>
+      <c r="D98" t="s">
+        <v>95</v>
+      </c>
+      <c r="E98" t="s">
+        <v>431</v>
+      </c>
+      <c r="G98" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>107</v>
+      </c>
+      <c r="B99" t="s">
+        <v>106</v>
+      </c>
+      <c r="C99" t="s">
+        <v>106</v>
+      </c>
+      <c r="D99" t="s">
+        <v>107</v>
+      </c>
+      <c r="E99" t="s">
+        <v>431</v>
+      </c>
+      <c r="G99" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -8339,10 +9367,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8386,9 +9414,6 @@
       <c r="E2" t="s">
         <v>431</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2" t="s">
         <v>316</v>
       </c>
@@ -8409,9 +9434,6 @@
       <c r="E3" t="s">
         <v>431</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
       <c r="G3" t="s">
         <v>318</v>
       </c>
@@ -8432,9 +9454,6 @@
       <c r="E4" t="s">
         <v>100</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
       <c r="G4" t="s">
         <v>319</v>
       </c>
@@ -8455,9 +9474,6 @@
       <c r="E5" t="s">
         <v>100</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
       <c r="G5" t="s">
         <v>433</v>
       </c>
@@ -8478,9 +9494,6 @@
       <c r="E6" t="s">
         <v>100</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
       <c r="G6" t="s">
         <v>320</v>
       </c>
@@ -8501,9 +9514,6 @@
       <c r="E7" t="s">
         <v>100</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
       <c r="G7" t="s">
         <v>321</v>
       </c>
@@ -8524,9 +9534,6 @@
       <c r="E8" t="s">
         <v>431</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
       <c r="G8" t="s">
         <v>323</v>
       </c>
@@ -8547,9 +9554,6 @@
       <c r="E9" t="s">
         <v>431</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
       <c r="G9" t="s">
         <v>325</v>
       </c>
@@ -9664,6 +10668,26 @@
       </c>
       <c r="G58" t="s">
         <v>610</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" t="s">
+        <v>94</v>
+      </c>
+      <c r="D59" t="s">
+        <v>95</v>
+      </c>
+      <c r="E59" t="s">
+        <v>431</v>
+      </c>
+      <c r="G59" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -9679,6 +10703,2559 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I90"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="7" max="7" width="52.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>1225</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>431</v>
+      </c>
+      <c r="F2" t="s">
+        <v>943</v>
+      </c>
+      <c r="G2" t="s">
+        <v>318</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" t="s">
+        <v>943</v>
+      </c>
+      <c r="G3" t="s">
+        <v>316</v>
+      </c>
+      <c r="I3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>943</v>
+      </c>
+      <c r="G4" t="s">
+        <v>317</v>
+      </c>
+      <c r="I4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>432</v>
+      </c>
+      <c r="B5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C5" t="s">
+        <v>432</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" t="s">
+        <v>944</v>
+      </c>
+      <c r="G5" t="s">
+        <v>433</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" t="s">
+        <v>944</v>
+      </c>
+      <c r="G6" t="s">
+        <v>320</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>945</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>945</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" t="s">
+        <v>944</v>
+      </c>
+      <c r="G7" t="s">
+        <v>321</v>
+      </c>
+      <c r="H7" t="s">
+        <v>946</v>
+      </c>
+      <c r="I7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>947</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>947</v>
+      </c>
+      <c r="D8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" t="s">
+        <v>431</v>
+      </c>
+      <c r="F8" t="s">
+        <v>943</v>
+      </c>
+      <c r="G8" t="s">
+        <v>322</v>
+      </c>
+      <c r="I8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>948</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" t="s">
+        <v>948</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>431</v>
+      </c>
+      <c r="F9" t="s">
+        <v>943</v>
+      </c>
+      <c r="G9" t="s">
+        <v>323</v>
+      </c>
+      <c r="I9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>949</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C10" t="s">
+        <v>949</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E10" t="s">
+        <v>431</v>
+      </c>
+      <c r="F10" t="s">
+        <v>943</v>
+      </c>
+      <c r="G10" t="s">
+        <v>950</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E11" t="s">
+        <v>431</v>
+      </c>
+      <c r="F11" t="s">
+        <v>943</v>
+      </c>
+      <c r="G11" t="s">
+        <v>951</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>952</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C12" t="s">
+        <v>952</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E12" t="s">
+        <v>430</v>
+      </c>
+      <c r="F12" t="s">
+        <v>954</v>
+      </c>
+      <c r="G12" t="s">
+        <v>953</v>
+      </c>
+      <c r="H12" t="s">
+        <v>955</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>956</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C13" t="s">
+        <v>956</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E13" t="s">
+        <v>430</v>
+      </c>
+      <c r="F13" t="s">
+        <v>954</v>
+      </c>
+      <c r="G13" t="s">
+        <v>957</v>
+      </c>
+      <c r="H13" t="s">
+        <v>955</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>958</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C14" t="s">
+        <v>958</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E14" t="s">
+        <v>430</v>
+      </c>
+      <c r="F14" t="s">
+        <v>954</v>
+      </c>
+      <c r="G14" t="s">
+        <v>959</v>
+      </c>
+      <c r="H14" t="s">
+        <v>955</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E15" t="s">
+        <v>430</v>
+      </c>
+      <c r="F15" t="s">
+        <v>954</v>
+      </c>
+      <c r="G15" t="s">
+        <v>960</v>
+      </c>
+      <c r="H15" t="s">
+        <v>955</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E16" t="s">
+        <v>430</v>
+      </c>
+      <c r="F16" t="s">
+        <v>954</v>
+      </c>
+      <c r="G16" t="s">
+        <v>961</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E17" t="s">
+        <v>430</v>
+      </c>
+      <c r="F17" t="s">
+        <v>954</v>
+      </c>
+      <c r="G17" t="s">
+        <v>962</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E18" t="s">
+        <v>430</v>
+      </c>
+      <c r="F18" t="s">
+        <v>954</v>
+      </c>
+      <c r="G18" t="s">
+        <v>963</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E19" t="s">
+        <v>430</v>
+      </c>
+      <c r="F19" t="s">
+        <v>954</v>
+      </c>
+      <c r="G19" t="s">
+        <v>964</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E20" t="s">
+        <v>430</v>
+      </c>
+      <c r="F20" t="s">
+        <v>954</v>
+      </c>
+      <c r="G20" t="s">
+        <v>965</v>
+      </c>
+      <c r="H20" t="s">
+        <v>966</v>
+      </c>
+      <c r="I20" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E21" t="s">
+        <v>430</v>
+      </c>
+      <c r="F21" t="s">
+        <v>954</v>
+      </c>
+      <c r="G21" t="s">
+        <v>967</v>
+      </c>
+      <c r="H21" t="s">
+        <v>968</v>
+      </c>
+      <c r="I21" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E22" t="s">
+        <v>430</v>
+      </c>
+      <c r="F22" t="s">
+        <v>954</v>
+      </c>
+      <c r="G22" t="s">
+        <v>969</v>
+      </c>
+      <c r="H22" t="s">
+        <v>970</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E23" t="s">
+        <v>430</v>
+      </c>
+      <c r="F23" t="s">
+        <v>954</v>
+      </c>
+      <c r="G23" t="s">
+        <v>971</v>
+      </c>
+      <c r="H23" t="s">
+        <v>972</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C24" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E24" t="s">
+        <v>430</v>
+      </c>
+      <c r="F24" t="s">
+        <v>954</v>
+      </c>
+      <c r="G24" t="s">
+        <v>973</v>
+      </c>
+      <c r="H24" t="s">
+        <v>974</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C25" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E25" t="s">
+        <v>430</v>
+      </c>
+      <c r="F25" t="s">
+        <v>954</v>
+      </c>
+      <c r="G25" t="s">
+        <v>975</v>
+      </c>
+      <c r="H25" t="s">
+        <v>976</v>
+      </c>
+      <c r="I25" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C26" t="s">
+        <v>132</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E26" t="s">
+        <v>430</v>
+      </c>
+      <c r="F26" t="s">
+        <v>954</v>
+      </c>
+      <c r="G26" t="s">
+        <v>977</v>
+      </c>
+      <c r="H26" t="s">
+        <v>978</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C27" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" t="s">
+        <v>896</v>
+      </c>
+      <c r="E27" t="s">
+        <v>430</v>
+      </c>
+      <c r="F27" t="s">
+        <v>954</v>
+      </c>
+      <c r="G27" t="s">
+        <v>979</v>
+      </c>
+      <c r="H27" t="s">
+        <v>980</v>
+      </c>
+      <c r="I27" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C28" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" t="s">
+        <v>897</v>
+      </c>
+      <c r="E28" t="s">
+        <v>430</v>
+      </c>
+      <c r="F28" t="s">
+        <v>954</v>
+      </c>
+      <c r="G28" t="s">
+        <v>981</v>
+      </c>
+      <c r="H28" t="s">
+        <v>982</v>
+      </c>
+      <c r="I28" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C29" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E29" t="s">
+        <v>430</v>
+      </c>
+      <c r="F29" t="s">
+        <v>954</v>
+      </c>
+      <c r="G29" t="s">
+        <v>983</v>
+      </c>
+      <c r="H29" t="s">
+        <v>984</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1166</v>
+      </c>
+      <c r="E30" t="s">
+        <v>430</v>
+      </c>
+      <c r="F30" t="s">
+        <v>954</v>
+      </c>
+      <c r="G30" t="s">
+        <v>985</v>
+      </c>
+      <c r="H30" t="s">
+        <v>986</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C31" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E31" t="s">
+        <v>430</v>
+      </c>
+      <c r="F31" t="s">
+        <v>954</v>
+      </c>
+      <c r="G31" t="s">
+        <v>987</v>
+      </c>
+      <c r="H31" t="s">
+        <v>988</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C32" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E32" t="s">
+        <v>430</v>
+      </c>
+      <c r="F32" t="s">
+        <v>954</v>
+      </c>
+      <c r="G32" t="s">
+        <v>989</v>
+      </c>
+      <c r="H32" t="s">
+        <v>990</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C33" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E33" t="s">
+        <v>430</v>
+      </c>
+      <c r="F33" t="s">
+        <v>954</v>
+      </c>
+      <c r="G33" t="s">
+        <v>991</v>
+      </c>
+      <c r="H33" t="s">
+        <v>992</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C34" t="s">
+        <v>148</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E34" t="s">
+        <v>430</v>
+      </c>
+      <c r="F34" t="s">
+        <v>954</v>
+      </c>
+      <c r="G34" t="s">
+        <v>993</v>
+      </c>
+      <c r="H34" t="s">
+        <v>994</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C35" t="s">
+        <v>150</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E35" t="s">
+        <v>430</v>
+      </c>
+      <c r="F35" t="s">
+        <v>954</v>
+      </c>
+      <c r="G35" t="s">
+        <v>995</v>
+      </c>
+      <c r="H35" t="s">
+        <v>996</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>152</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C36" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E36" t="s">
+        <v>430</v>
+      </c>
+      <c r="F36" t="s">
+        <v>954</v>
+      </c>
+      <c r="G36" t="s">
+        <v>997</v>
+      </c>
+      <c r="H36" t="s">
+        <v>998</v>
+      </c>
+      <c r="I36" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C37" t="s">
+        <v>154</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E37" t="s">
+        <v>430</v>
+      </c>
+      <c r="F37" t="s">
+        <v>954</v>
+      </c>
+      <c r="G37" t="s">
+        <v>999</v>
+      </c>
+      <c r="H37" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I37" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>156</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C38" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E38" t="s">
+        <v>430</v>
+      </c>
+      <c r="F38" t="s">
+        <v>954</v>
+      </c>
+      <c r="G38" t="s">
+        <v>1001</v>
+      </c>
+      <c r="H38" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I38" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>158</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E39" t="s">
+        <v>430</v>
+      </c>
+      <c r="F39" t="s">
+        <v>954</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H39" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I39" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>160</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C40" t="s">
+        <v>160</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1176</v>
+      </c>
+      <c r="E40" t="s">
+        <v>430</v>
+      </c>
+      <c r="F40" t="s">
+        <v>954</v>
+      </c>
+      <c r="G40" t="s">
+        <v>1005</v>
+      </c>
+      <c r="H40" t="s">
+        <v>1006</v>
+      </c>
+      <c r="I40" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>162</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C41" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E41" t="s">
+        <v>430</v>
+      </c>
+      <c r="F41" t="s">
+        <v>954</v>
+      </c>
+      <c r="G41" t="s">
+        <v>1007</v>
+      </c>
+      <c r="H41" t="s">
+        <v>1008</v>
+      </c>
+      <c r="I41" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>164</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C42" t="s">
+        <v>164</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E42" t="s">
+        <v>430</v>
+      </c>
+      <c r="F42" t="s">
+        <v>954</v>
+      </c>
+      <c r="G42" t="s">
+        <v>1009</v>
+      </c>
+      <c r="H42" t="s">
+        <v>1010</v>
+      </c>
+      <c r="I42" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E43" t="s">
+        <v>430</v>
+      </c>
+      <c r="F43" t="s">
+        <v>954</v>
+      </c>
+      <c r="G43" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H43" t="s">
+        <v>1012</v>
+      </c>
+      <c r="I43" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>168</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C44" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E44" t="s">
+        <v>430</v>
+      </c>
+      <c r="F44" t="s">
+        <v>954</v>
+      </c>
+      <c r="G44" t="s">
+        <v>1013</v>
+      </c>
+      <c r="H44" t="s">
+        <v>1014</v>
+      </c>
+      <c r="I44" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>170</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C45" t="s">
+        <v>170</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E45" t="s">
+        <v>430</v>
+      </c>
+      <c r="F45" t="s">
+        <v>954</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H45" t="s">
+        <v>1016</v>
+      </c>
+      <c r="I45" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C46" t="s">
+        <v>172</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E46" t="s">
+        <v>430</v>
+      </c>
+      <c r="F46" t="s">
+        <v>954</v>
+      </c>
+      <c r="G46" t="s">
+        <v>1017</v>
+      </c>
+      <c r="H46" t="s">
+        <v>1018</v>
+      </c>
+      <c r="I46" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>174</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C47" t="s">
+        <v>174</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E47" t="s">
+        <v>430</v>
+      </c>
+      <c r="F47" t="s">
+        <v>954</v>
+      </c>
+      <c r="G47" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H47" t="s">
+        <v>1020</v>
+      </c>
+      <c r="I47" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>176</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C48" t="s">
+        <v>176</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E48" t="s">
+        <v>430</v>
+      </c>
+      <c r="F48" t="s">
+        <v>954</v>
+      </c>
+      <c r="G48" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H48" t="s">
+        <v>1022</v>
+      </c>
+      <c r="I48" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C49" t="s">
+        <v>178</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E49" t="s">
+        <v>430</v>
+      </c>
+      <c r="F49" t="s">
+        <v>954</v>
+      </c>
+      <c r="G49" t="s">
+        <v>1023</v>
+      </c>
+      <c r="H49" t="s">
+        <v>1024</v>
+      </c>
+      <c r="I49" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>180</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C50" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E50" t="s">
+        <v>430</v>
+      </c>
+      <c r="F50" t="s">
+        <v>954</v>
+      </c>
+      <c r="G50" t="s">
+        <v>1025</v>
+      </c>
+      <c r="H50" t="s">
+        <v>1026</v>
+      </c>
+      <c r="I50" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
+        <v>182</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C51" t="s">
+        <v>182</v>
+      </c>
+      <c r="D51" t="s">
+        <v>918</v>
+      </c>
+      <c r="E51" t="s">
+        <v>430</v>
+      </c>
+      <c r="F51" t="s">
+        <v>954</v>
+      </c>
+      <c r="G51" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H51" t="s">
+        <v>1028</v>
+      </c>
+      <c r="I51" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>184</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C52" t="s">
+        <v>184</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E52" t="s">
+        <v>430</v>
+      </c>
+      <c r="F52" t="s">
+        <v>954</v>
+      </c>
+      <c r="G52" t="s">
+        <v>1029</v>
+      </c>
+      <c r="H52" t="s">
+        <v>1030</v>
+      </c>
+      <c r="I52" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>186</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C53" t="s">
+        <v>186</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E53" t="s">
+        <v>430</v>
+      </c>
+      <c r="F53" t="s">
+        <v>954</v>
+      </c>
+      <c r="G53" t="s">
+        <v>1031</v>
+      </c>
+      <c r="H53" t="s">
+        <v>1032</v>
+      </c>
+      <c r="I53" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>190</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C54" t="s">
+        <v>190</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E54" t="s">
+        <v>430</v>
+      </c>
+      <c r="F54" t="s">
+        <v>954</v>
+      </c>
+      <c r="G54" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H54" t="s">
+        <v>1034</v>
+      </c>
+      <c r="I54" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C55" t="s">
+        <v>192</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E55" t="s">
+        <v>430</v>
+      </c>
+      <c r="F55" t="s">
+        <v>954</v>
+      </c>
+      <c r="G55" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H55" t="s">
+        <v>1036</v>
+      </c>
+      <c r="I55" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>194</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C56" t="s">
+        <v>194</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E56" t="s">
+        <v>430</v>
+      </c>
+      <c r="F56" t="s">
+        <v>954</v>
+      </c>
+      <c r="G56" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H56" t="s">
+        <v>1038</v>
+      </c>
+      <c r="I56" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>196</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C57" t="s">
+        <v>196</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E57" t="s">
+        <v>430</v>
+      </c>
+      <c r="F57" t="s">
+        <v>954</v>
+      </c>
+      <c r="G57" t="s">
+        <v>1039</v>
+      </c>
+      <c r="H57" t="s">
+        <v>1040</v>
+      </c>
+      <c r="I57" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>198</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C58" t="s">
+        <v>198</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E58" t="s">
+        <v>430</v>
+      </c>
+      <c r="F58" t="s">
+        <v>954</v>
+      </c>
+      <c r="G58" t="s">
+        <v>1041</v>
+      </c>
+      <c r="H58" t="s">
+        <v>1042</v>
+      </c>
+      <c r="I58" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>200</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C59" t="s">
+        <v>200</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E59" t="s">
+        <v>430</v>
+      </c>
+      <c r="F59" t="s">
+        <v>954</v>
+      </c>
+      <c r="G59" t="s">
+        <v>1043</v>
+      </c>
+      <c r="H59" t="s">
+        <v>1044</v>
+      </c>
+      <c r="I59" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>202</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C60" t="s">
+        <v>202</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E60" t="s">
+        <v>430</v>
+      </c>
+      <c r="F60" t="s">
+        <v>954</v>
+      </c>
+      <c r="G60" t="s">
+        <v>1045</v>
+      </c>
+      <c r="H60" t="s">
+        <v>1046</v>
+      </c>
+      <c r="I60" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>204</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C61" t="s">
+        <v>204</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1198</v>
+      </c>
+      <c r="E61" t="s">
+        <v>430</v>
+      </c>
+      <c r="F61" t="s">
+        <v>954</v>
+      </c>
+      <c r="G61" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H61" t="s">
+        <v>1048</v>
+      </c>
+      <c r="I61" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>206</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C62" t="s">
+        <v>206</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E62" t="s">
+        <v>430</v>
+      </c>
+      <c r="F62" t="s">
+        <v>954</v>
+      </c>
+      <c r="G62" t="s">
+        <v>1049</v>
+      </c>
+      <c r="H62" t="s">
+        <v>1050</v>
+      </c>
+      <c r="I62" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>208</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C63" t="s">
+        <v>208</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E63" t="s">
+        <v>430</v>
+      </c>
+      <c r="F63" t="s">
+        <v>954</v>
+      </c>
+      <c r="G63" t="s">
+        <v>1051</v>
+      </c>
+      <c r="H63" t="s">
+        <v>1052</v>
+      </c>
+      <c r="I63" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>210</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C64" t="s">
+        <v>210</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E64" t="s">
+        <v>430</v>
+      </c>
+      <c r="F64" t="s">
+        <v>954</v>
+      </c>
+      <c r="G64" t="s">
+        <v>1053</v>
+      </c>
+      <c r="H64" t="s">
+        <v>1054</v>
+      </c>
+      <c r="I64" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>212</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C65" t="s">
+        <v>212</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E65" t="s">
+        <v>430</v>
+      </c>
+      <c r="F65" t="s">
+        <v>954</v>
+      </c>
+      <c r="G65" t="s">
+        <v>1055</v>
+      </c>
+      <c r="H65" t="s">
+        <v>1056</v>
+      </c>
+      <c r="I65" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>214</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C66" t="s">
+        <v>214</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E66" t="s">
+        <v>430</v>
+      </c>
+      <c r="F66" t="s">
+        <v>954</v>
+      </c>
+      <c r="G66" t="s">
+        <v>1057</v>
+      </c>
+      <c r="H66" t="s">
+        <v>1058</v>
+      </c>
+      <c r="I66" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>216</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C67" t="s">
+        <v>216</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1204</v>
+      </c>
+      <c r="E67" t="s">
+        <v>430</v>
+      </c>
+      <c r="F67" t="s">
+        <v>954</v>
+      </c>
+      <c r="G67" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H67" t="s">
+        <v>1060</v>
+      </c>
+      <c r="I67" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>218</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C68" t="s">
+        <v>218</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1205</v>
+      </c>
+      <c r="E68" t="s">
+        <v>430</v>
+      </c>
+      <c r="F68" t="s">
+        <v>954</v>
+      </c>
+      <c r="G68" t="s">
+        <v>1061</v>
+      </c>
+      <c r="H68" t="s">
+        <v>1062</v>
+      </c>
+      <c r="I68" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>220</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C69" t="s">
+        <v>220</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E69" t="s">
+        <v>430</v>
+      </c>
+      <c r="F69" t="s">
+        <v>954</v>
+      </c>
+      <c r="G69" t="s">
+        <v>1063</v>
+      </c>
+      <c r="H69" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I69" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>222</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C70" t="s">
+        <v>222</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E70" t="s">
+        <v>430</v>
+      </c>
+      <c r="F70" t="s">
+        <v>954</v>
+      </c>
+      <c r="G70" t="s">
+        <v>1065</v>
+      </c>
+      <c r="H70" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I70" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>224</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C71" t="s">
+        <v>224</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1208</v>
+      </c>
+      <c r="E71" t="s">
+        <v>430</v>
+      </c>
+      <c r="F71" t="s">
+        <v>954</v>
+      </c>
+      <c r="G71" t="s">
+        <v>1067</v>
+      </c>
+      <c r="H71" t="s">
+        <v>1068</v>
+      </c>
+      <c r="I71" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>226</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C72" t="s">
+        <v>226</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1209</v>
+      </c>
+      <c r="E72" t="s">
+        <v>430</v>
+      </c>
+      <c r="F72" t="s">
+        <v>954</v>
+      </c>
+      <c r="G72" t="s">
+        <v>1069</v>
+      </c>
+      <c r="H72" t="s">
+        <v>1070</v>
+      </c>
+      <c r="I72" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>234</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C73" t="s">
+        <v>234</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E73" t="s">
+        <v>430</v>
+      </c>
+      <c r="F73" t="s">
+        <v>954</v>
+      </c>
+      <c r="G73" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H73" t="s">
+        <v>1072</v>
+      </c>
+      <c r="I73" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>230</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C74" t="s">
+        <v>230</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E74" t="s">
+        <v>430</v>
+      </c>
+      <c r="F74" t="s">
+        <v>954</v>
+      </c>
+      <c r="G74" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H74" t="s">
+        <v>1074</v>
+      </c>
+      <c r="I74" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" t="s">
+        <v>238</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C75" t="s">
+        <v>238</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1212</v>
+      </c>
+      <c r="E75" t="s">
+        <v>430</v>
+      </c>
+      <c r="F75" t="s">
+        <v>954</v>
+      </c>
+      <c r="G75" t="s">
+        <v>1075</v>
+      </c>
+      <c r="H75" t="s">
+        <v>1074</v>
+      </c>
+      <c r="I75" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" t="s">
+        <v>240</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C76" t="s">
+        <v>240</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1213</v>
+      </c>
+      <c r="E76" t="s">
+        <v>430</v>
+      </c>
+      <c r="F76" t="s">
+        <v>954</v>
+      </c>
+      <c r="G76" t="s">
+        <v>1076</v>
+      </c>
+      <c r="H76" t="s">
+        <v>1074</v>
+      </c>
+      <c r="I76" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" t="s">
+        <v>232</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C77" t="s">
+        <v>232</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1214</v>
+      </c>
+      <c r="E77" t="s">
+        <v>430</v>
+      </c>
+      <c r="F77" t="s">
+        <v>954</v>
+      </c>
+      <c r="G77" t="s">
+        <v>1077</v>
+      </c>
+      <c r="I77" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" t="s">
+        <v>254</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C78" t="s">
+        <v>254</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E78" t="s">
+        <v>430</v>
+      </c>
+      <c r="F78" t="s">
+        <v>954</v>
+      </c>
+      <c r="G78" t="s">
+        <v>1078</v>
+      </c>
+      <c r="I78" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" t="s">
+        <v>256</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C79" t="s">
+        <v>256</v>
+      </c>
+      <c r="D79" t="s">
+        <v>850</v>
+      </c>
+      <c r="E79" t="s">
+        <v>430</v>
+      </c>
+      <c r="F79" t="s">
+        <v>954</v>
+      </c>
+      <c r="G79" t="s">
+        <v>1239</v>
+      </c>
+      <c r="I79" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" t="s">
+        <v>258</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C80" t="s">
+        <v>258</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E80" t="s">
+        <v>430</v>
+      </c>
+      <c r="F80" t="s">
+        <v>954</v>
+      </c>
+      <c r="G80" t="s">
+        <v>1216</v>
+      </c>
+      <c r="I80" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" t="s">
+        <v>260</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C81" t="s">
+        <v>260</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1217</v>
+      </c>
+      <c r="E81" t="s">
+        <v>430</v>
+      </c>
+      <c r="F81" t="s">
+        <v>954</v>
+      </c>
+      <c r="G81" t="s">
+        <v>1217</v>
+      </c>
+      <c r="I81" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" t="s">
+        <v>262</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C82" t="s">
+        <v>262</v>
+      </c>
+      <c r="D82" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E82" t="s">
+        <v>430</v>
+      </c>
+      <c r="F82" t="s">
+        <v>954</v>
+      </c>
+      <c r="G82" t="s">
+        <v>1161</v>
+      </c>
+      <c r="I82" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" t="s">
+        <v>264</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C83" t="s">
+        <v>264</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E83" t="s">
+        <v>430</v>
+      </c>
+      <c r="F83" t="s">
+        <v>954</v>
+      </c>
+      <c r="G83" t="s">
+        <v>1218</v>
+      </c>
+      <c r="I83" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" t="s">
+        <v>266</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C84" t="s">
+        <v>266</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1219</v>
+      </c>
+      <c r="E84" t="s">
+        <v>430</v>
+      </c>
+      <c r="F84" t="s">
+        <v>954</v>
+      </c>
+      <c r="G84" t="s">
+        <v>1219</v>
+      </c>
+      <c r="I84" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" t="s">
+        <v>268</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C85" t="s">
+        <v>268</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1220</v>
+      </c>
+      <c r="E85" t="s">
+        <v>430</v>
+      </c>
+      <c r="F85" t="s">
+        <v>954</v>
+      </c>
+      <c r="G85" t="s">
+        <v>1220</v>
+      </c>
+      <c r="I85" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" t="s">
+        <v>270</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C86" t="s">
+        <v>270</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1221</v>
+      </c>
+      <c r="E86" t="s">
+        <v>430</v>
+      </c>
+      <c r="F86" t="s">
+        <v>954</v>
+      </c>
+      <c r="G86" t="s">
+        <v>1221</v>
+      </c>
+      <c r="I86" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" t="s">
+        <v>272</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C87" t="s">
+        <v>272</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1222</v>
+      </c>
+      <c r="E87" t="s">
+        <v>430</v>
+      </c>
+      <c r="F87" t="s">
+        <v>954</v>
+      </c>
+      <c r="G87" t="s">
+        <v>1222</v>
+      </c>
+      <c r="I87" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" t="s">
+        <v>274</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C88" t="s">
+        <v>274</v>
+      </c>
+      <c r="D88" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E88" t="s">
+        <v>430</v>
+      </c>
+      <c r="F88" t="s">
+        <v>954</v>
+      </c>
+      <c r="G88" t="s">
+        <v>1223</v>
+      </c>
+      <c r="I88" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" t="s">
+        <v>276</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C89" t="s">
+        <v>276</v>
+      </c>
+      <c r="D89" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E89" t="s">
+        <v>430</v>
+      </c>
+      <c r="F89" t="s">
+        <v>954</v>
+      </c>
+      <c r="G89" t="s">
+        <v>1224</v>
+      </c>
+      <c r="I89" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" t="s">
+        <v>188</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C90" t="s">
+        <v>188</v>
+      </c>
+      <c r="D90" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E90" t="s">
+        <v>430</v>
+      </c>
+      <c r="F90" t="s">
+        <v>954</v>
+      </c>
+      <c r="G90" t="s">
+        <v>1189</v>
+      </c>
+      <c r="I90" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>

</xml_diff>